<commit_message>
Dossier : Syntagmes & Patrons amélioré, 3 Patrons fait
</commit_message>
<xml_diff>
--- a/dossiers/Final - Références articles.xlsx
+++ b/dossiers/Final - Références articles.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79E73B-E3CA-4EA1-86D6-4D09D0B21624}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Citations" sheetId="3" r:id="rId4"/>
     <sheet name="Retrouver" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="225">
   <si>
     <t>Gross, M. (1994). Dictionnaires électroniques et traduction automatique. Langages, 48-58.</t>
   </si>
@@ -166,10 +167,6 @@
   </si>
   <si>
     <t>Rastier</t>
-  </si>
-  <si>
-    <t>3 dicho : langue/parole=prodlang, signifiant/signifié=concept mental, diachro/synchro
-chapitre IV pour la définition de la dicho lang/parole</t>
   </si>
   <si>
     <t>Morpho</t>
@@ -513,9 +510,6 @@
   </si>
   <si>
     <t>Gadet</t>
-  </si>
-  <si>
-    <t>paradoxe de l'observateur : celui-ci souhaite observer ce qui se passe quand il n’est pas là.</t>
   </si>
   <si>
     <t>ExoSDL (oublié)
@@ -1808,9 +1802,6 @@
     </r>
   </si>
   <si>
-    <t>« En raison de sa finitude, le corpus ne réalise donc qu'une part infime de ce qui est réalisable. (…) Et en toute rigueur, une grammaire construite à partir d'un corpus ne vaut que pour le corpus qui l'a produite. »</t>
-  </si>
-  <si>
     <r>
       <t>Sagot, B. (2010, May). The Lefff, a freely available and large-coverage morphological and syntactic lexicon for French. In </t>
     </r>
@@ -1958,13 +1949,337 @@
   </si>
   <si>
     <t>Les inexactitudes dans les titres : les trucs pas bien selon lui</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Legallois, D. (2006). II-3 Pattern Grammar. Dans D. Legallois, &amp; J. François, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Autour des grammaires de constructions et de patterns. Cahier du CRISCO, 21.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (pp. 33-42). Caen: Centre de Recherches Interlangues sur la Signification en Contexte.</t>
+    </r>
+  </si>
+  <si>
+    <t>MémRech II</t>
+  </si>
+  <si>
+    <t>Legallois</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <r>
+      <t>Johnson, C. (2001). Book Reviews: Pattern Grammar: A Corpus-Driven Approach to the Lexical Grammar of English. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Computational Linguistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2).</t>
+    </r>
+  </si>
+  <si>
+    <t>Johnson (note de lecture de Hunston &amp; Francis)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Décrit le livre introuvable de Hunston &amp; Francis (pattern grammar, contextualiste) :
+Ils définissent un truc aussi générique que V n
+Corpus data &gt; introspection (c'est du driven car peu présupposés théoriques)
+Corpus driven : très peu de présupposé théorique (vs corpus based)
+Trouve ses racines dans :
+    - les descriptions pédagogiques du langages : Hornby 1954
+    - le travail sur corpus de Sinclair 1991
+Mais pas de théorie globale et de définition formelle des patrons.
+COMLEX syntax évoqué : projet de Macleod, Grishman, Meyers, 1998
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La distinction lexique / grammaire s'efface car les lexèmes s'inscrivent dans des patterns grammaticaux</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comparaison de [Grammaire de construction &lt;- L cognitive ] vs 
+  [Grammaire de patrons/patrons](association fréquente entre un mot cible +d'autres mots)
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> La structure syntaxique (= grammaire) entière possède un sens (et plus seulement les lexèmes)
+    Ce sens est-il inférenciel ou immanent ?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  Patron indépendant des syntagmes
+  Perspective didactique et descriptive
+  Parle des shell noun : noms sous-spécifiés sémantiquement HJ Schmid 2000
+  Utilise un gros corpus Bank of English (300 millions de mots)
+  Sinclair puis Hunston et Francis (qui ont fait le COBUILD)
+Grammaire = réseau de constructons vs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Grammaire = accumulation de patrons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enfin, parle de Hoey (2005) et l'amorçage/lexical priming : un mot en appel un autre.
+"un lexème est acquis grâce à ses occurrences dans les discours et textes, il se charge cumulativement des contextes et des co-textes dans lesquels il est "rencontré".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>paradoxe de l'observateur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : celui-ci souhaite observer ce qui se passe quand il n’est pas là.
+Mais finalement, celui-ci postule qu'il y a une situation SANS modification, "PURE", dans une perspective positiviste… = "une réalité neutre, indépendante de la perspective prise par l'observateur"
+Astuce pour contourner le paradoxe. Mais attention à aller "trop loin" (espionnage) : interview, groupe de parole...
+Labov (82) et Milroy (87) =&gt; deux grands noms de l'enquête sociolinguistique
+Cameron Deborah (1992-1993) va très loin : il faut, outre une démarche Éthique (sur eux), défendre (pour eux) et même empowerer (avec eux) les personnes de notre sujet d'étude.
+Ex : auto-commentaire des interrogés sur leur discours
+! différence entre ceux que l'on sait et ce que l'on fait dans ces questions...
+Dans tous les cas, le sujet de notre étude, ce sont des personnes avec la considération éthique, politique et sociale nécessaire.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Townsend</t>
+  </si>
+  <si>
+    <t>Reprend Dillon (1981) qui mettait en relation la présence d'un colon avec la publication :
+il comparait 474 titres non publiés vs 314 titres publiés
+Townsend fait de même avec des journaux néo-zélandais :
+OK, pour le rapport publié / non publié
+Par contre, faible relation avec l'impact mesuré par nombre de citations.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Townsend, M. A. (1983). Titular Colonicity and Scholarship: New Zealand Research and Scholarly Impact. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Zealand Journal of Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 41-43.</t>
+    </r>
+  </si>
+  <si>
+    <t>« En raison de sa finitude, le corpus ne réalise donc qu'une part infime de ce qui est réalisable. (…)
+Et en toute rigueur, une grammaire construite à partir d'un corpus ne vaut que pour le corpus qui l'a produite. »</t>
+  </si>
+  <si>
+    <t>3 dicho : langue/parole=prodlang, signifiant/signifié=concept mental, diachro/synchro
+chapitre IV pour la définition de la dicho lang/parole
+&gt; ne pas oublier de rajouter le "référant", venu + tard, la chose du monde, à signifiant/signifié.</t>
+  </si>
+  <si>
+    <t>Nagano</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nagano, R. L. (2015). Research article titles and disciplinary conventions: A corpus study of eight disciplines. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Journal of Academic Writing, 5(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 133-144.</t>
+    </r>
+  </si>
+  <si>
+    <t>MR12</t>
+  </si>
+  <si>
+    <t>MR11</t>
+  </si>
+  <si>
+    <t>MR10</t>
+  </si>
+  <si>
+    <t>MR9</t>
+  </si>
+  <si>
+    <t>MR8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Substantive word rate (nombre de nom / nombre de mots) : 
+« ce taux est souvent considéré comme un indicateur pour déterminer combien ce titre est informatif »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+décide de traiter les partitions séparément et ramènent celles-ci à deux titres indépendants, l’un étant le titre, l’autre le sous-titre. 
+Hard sciences / soft sciences
+hard sciences : +mots +noun phrase +substantive word rate -the au début
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étude du « the » au début</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2052,8 +2367,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2114,6 +2436,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2128,7 +2462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2223,6 +2557,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2545,1011 +2891,1293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7BB45F-7C76-4B6C-9D19-22CA475005CE}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="81" style="27" customWidth="1"/>
-    <col min="7" max="7" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="180" style="32" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="6.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="88" style="27" customWidth="1"/>
+    <col min="8" max="8" width="6" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="180" style="32" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="F1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="9">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="9">
-        <v>2014</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="G2" s="19">
+      <c r="E2" s="6"/>
+      <c r="F2" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="19">
         <v>10</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="16"/>
+      <c r="C3" s="7">
         <v>2003</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="6">
+      <c r="F3" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="6">
         <v>25</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="I3" s="34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="7">
+        <v>2002</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="8">
+        <v>1998</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="6">
+        <v>223</v>
+      </c>
+      <c r="I5" s="33" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2002</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="27" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="9">
+        <v>2017</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="6">
-        <v>9</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1998</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="6">
-        <v>223</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="9">
-        <v>2017</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="H6" s="6">
         <v>377</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="16"/>
+      <c r="C7" s="7">
         <v>2002</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6">
+      <c r="F7" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="6">
         <v>18</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I7" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="7">
+        <v>80</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="7">
         <v>2008</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="F8" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="6">
         <v>15</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="16"/>
+      <c r="C9" s="8">
         <v>1990</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="6">
+      <c r="F9" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="6">
         <v>179</v>
       </c>
-      <c r="H9" s="34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="16"/>
+      <c r="C10" s="7">
         <v>2004</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="6">
+      <c r="F10" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" s="6">
         <v>23</v>
       </c>
-      <c r="H10" s="34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="9">
+        <v>79</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="9">
         <v>2012</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="D12" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="6">
+      <c r="F12" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="H12" s="37">
         <v>12046</v>
       </c>
-      <c r="H12" s="34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="16"/>
+      <c r="C13" s="7">
         <v>2003</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="6">
+      <c r="F13" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="6">
         <v>105</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="I13" s="34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="8">
+        <v>1998</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="6">
+        <v>61</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="7">
+        <v>2005</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="6">
+        <v>5</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2003</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" s="6">
+        <v>49</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="7">
+        <v>2009</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="6">
+        <v>170</v>
+      </c>
+      <c r="I17" s="34" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1998</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="G14" s="6">
-        <v>61</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="7">
-        <v>2005</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="6">
-        <v>5</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="7">
-        <v>2003</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="G16" s="6">
-        <v>49</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="270" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="7">
-        <v>2009</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="G17" s="6">
-        <v>170</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="16"/>
+      <c r="C18" s="8">
         <v>1994</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="F18" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I18" s="32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="16"/>
+      <c r="C19" s="8">
         <v>1997</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="G19" s="6">
+      <c r="F19" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="6">
         <v>504</v>
       </c>
-      <c r="H19" s="34" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="7">
+        <v>84</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="7">
         <v>2004</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="D20" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="6">
         <v>160</v>
       </c>
-      <c r="H20" s="33" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="16"/>
+      <c r="C21" s="8">
         <v>1972</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="F21" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I21" s="32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="9">
+        <v>85</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="9">
         <v>2011</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="33" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="7">
-        <v>2002</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2001</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" s="6">
+        <v>22</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="16"/>
+      <c r="C24" s="7">
         <v>2002</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="7">
+        <v>2002</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24" s="32" t="s">
+      <c r="F25" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="7">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="7">
         <v>2001</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="D26" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" s="6">
+        <v>23</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" s="6">
+        <v>204</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" s="7">
+        <v>2006</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="H28" s="6">
+        <v>54</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="7">
+        <v>2006</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="6">
+        <v>21</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="7">
+        <v>2008</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H30" s="6">
+        <v>24</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H31" s="6">
+        <v>83</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8">
+        <v>1988</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="7">
+        <v>2002</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" s="6">
+        <v>488</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="8">
+        <v>1977</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="6">
+        <v>304</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="H37" s="6">
+        <v>9</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="16"/>
+      <c r="C39" s="7">
+        <v>2003</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" s="6">
+        <v>236</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="9">
+        <v>2017</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41" s="6">
+        <v>4</v>
+      </c>
+      <c r="I41" s="34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="6">
+      <c r="F42" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H42" s="6">
+        <v>207</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="7">
+        <v>2009</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H43" s="6">
+        <v>17</v>
+      </c>
+      <c r="I43" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="H44" s="6">
+        <v>176</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" s="6">
+        <v>3367</v>
+      </c>
+      <c r="I45" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="H46" s="6">
+        <v>3</v>
+      </c>
+      <c r="I46" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="8">
+        <v>1991</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="16"/>
+      <c r="C48" s="7">
+        <v>2004</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" s="37">
+        <v>1426</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" s="6">
+        <v>68</v>
+      </c>
+      <c r="I49" s="33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="16"/>
+      <c r="C50" s="7">
+        <v>2009</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="B26" s="7">
-        <v>2000</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="G26" s="6">
+      <c r="B51" s="16"/>
+      <c r="C51" s="8">
+        <v>1996</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" s="37">
+        <v>2055</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1983</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B27" s="7">
-        <v>2006</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" s="6">
-        <v>21</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="7">
-        <v>2008</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="F52" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="H52" s="6">
+        <v>10</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="16"/>
+      <c r="C53" s="9">
+        <v>2013</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="6">
-        <v>24</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="7">
+      <c r="F53" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="7">
+        <v>2004</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="6">
+        <v>16</v>
+      </c>
+      <c r="I54" s="33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="7">
         <v>2005</v>
       </c>
-      <c r="C29" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="6">
-        <v>83</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="8">
-        <v>1988</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="7">
-        <v>2002</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" t="s">
-        <v>192</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="7">
-        <v>2005</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="7">
-        <v>2005</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="G33" s="6">
-        <v>488</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8">
-        <v>1977</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="6">
-        <v>304</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="9">
-        <v>2010</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="7">
-        <v>2003</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="6">
-        <v>236</v>
-      </c>
-      <c r="H37" s="34" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="9">
-        <v>2017</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G38" s="6">
-        <v>4</v>
-      </c>
-      <c r="H38" s="34" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="7">
-        <v>2005</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="6">
-        <v>207</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="7">
-        <v>2009</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" s="6">
-        <v>17</v>
-      </c>
-      <c r="H40" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B41" s="9">
-        <v>2010</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="G41" s="6">
-        <v>176</v>
-      </c>
-      <c r="H41" s="33" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42" s="6">
-        <v>3367</v>
-      </c>
-      <c r="H42" s="33" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B43" s="9">
-        <v>2015</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="G43" s="6">
-        <v>3</v>
-      </c>
-      <c r="H43" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="8">
-        <v>1991</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H44" s="32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="7">
-        <v>2004</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="H45" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" s="9">
-        <v>2015</v>
-      </c>
-      <c r="C46" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="6">
-        <v>68</v>
-      </c>
-      <c r="H46" s="33" t="s">
+      <c r="D55" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="9">
+        <v>2012</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="G56" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+      <c r="I56" s="34" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="7">
-        <v>2009</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H47" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="8">
-        <v>1996</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B49" s="9">
-        <v>2013</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H49" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="7">
-        <v>2004</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G50" s="6">
-        <v>16</v>
-      </c>
-      <c r="H50" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="7">
-        <v>2005</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="H51" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="9">
-        <v>2012</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F52" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G52" s="6">
-        <v>0</v>
-      </c>
-      <c r="H52" s="34" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3577,16 +4205,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3606,84 +4234,84 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>2001</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2001</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>2000</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>1991</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3718,101 +4346,101 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
         <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
         <v>107</v>
-      </c>
-      <c r="B9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
         <v>112</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3835,18 +4463,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3869,43 +4497,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dossier : encore du travail sur résultats et perspectives.
En plus :
- Il reste la conclusion entière
- Traité les résultats des 2 patrons (SN CC SN fait)
</commit_message>
<xml_diff>
--- a/dossiers/Final - Références articles.xlsx
+++ b/dossiers/Final - Références articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79E73B-E3CA-4EA1-86D6-4D09D0B21624}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BF6E62-837D-4210-800B-93962B4E2AA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="242">
   <si>
     <t>Gross, M. (1994). Dictionnaires électroniques et traduction automatique. Langages, 48-58.</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Mayaffre, D. (2005). De la lexicométrie à la logométrie. Astrolabe, 1-11.</t>
-  </si>
-  <si>
-    <t>Sinclair, J. (1991). Corpus, concordance, collocation. Oxford University Press.</t>
   </si>
   <si>
     <t>Souvay, G., Pierrel, J. M. (2009). LGERM Lemmatisation des mots en Moyen Français. Traitement Automatique des Langues, 50 (2), 21.</t>
@@ -496,9 +493,6 @@
   </si>
   <si>
     <t>SOLR</t>
-  </si>
-  <si>
-    <t>Le web n'est pas un corpus : il évolue et n'est pas clos !</t>
   </si>
   <si>
     <t>Remise en cause dichotomie lang/parole ou comp/perf
@@ -2033,6 +2027,274 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>paradoxe de l'observateur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : celui-ci souhaite observer ce qui se passe quand il n’est pas là.
+Mais finalement, celui-ci postule qu'il y a une situation SANS modification, "PURE", dans une perspective positiviste… = "une réalité neutre, indépendante de la perspective prise par l'observateur"
+Astuce pour contourner le paradoxe. Mais attention à aller "trop loin" (espionnage) : interview, groupe de parole...
+Labov (82) et Milroy (87) =&gt; deux grands noms de l'enquête sociolinguistique
+Cameron Deborah (1992-1993) va très loin : il faut, outre une démarche Éthique (sur eux), défendre (pour eux) et même empowerer (avec eux) les personnes de notre sujet d'étude.
+Ex : auto-commentaire des interrogés sur leur discours
+! différence entre ceux que l'on sait et ce que l'on fait dans ces questions...
+Dans tous les cas, le sujet de notre étude, ce sont des personnes avec la considération éthique, politique et sociale nécessaire.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Townsend</t>
+  </si>
+  <si>
+    <t>Reprend Dillon (1981) qui mettait en relation la présence d'un colon avec la publication :
+il comparait 474 titres non publiés vs 314 titres publiés
+Townsend fait de même avec des journaux néo-zélandais :
+OK, pour le rapport publié / non publié
+Par contre, faible relation avec l'impact mesuré par nombre de citations.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Townsend, M. A. (1983). Titular Colonicity and Scholarship: New Zealand Research and Scholarly Impact. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Zealand Journal of Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 41-43.</t>
+    </r>
+  </si>
+  <si>
+    <t>« En raison de sa finitude, le corpus ne réalise donc qu'une part infime de ce qui est réalisable. (…)
+Et en toute rigueur, une grammaire construite à partir d'un corpus ne vaut que pour le corpus qui l'a produite. »</t>
+  </si>
+  <si>
+    <t>3 dicho : langue/parole=prodlang, signifiant/signifié=concept mental, diachro/synchro
+chapitre IV pour la définition de la dicho lang/parole
+&gt; ne pas oublier de rajouter le "référant", venu + tard, la chose du monde, à signifiant/signifié.</t>
+  </si>
+  <si>
+    <t>Nagano</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nagano, R. L. (2015). Research article titles and disciplinary conventions: A corpus study of eight disciplines. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Journal of Academic Writing, 5(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 133-144.</t>
+    </r>
+  </si>
+  <si>
+    <t>MR12</t>
+  </si>
+  <si>
+    <t>MR11</t>
+  </si>
+  <si>
+    <t>MR10</t>
+  </si>
+  <si>
+    <t>MR9</t>
+  </si>
+  <si>
+    <t>MR8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Substantive word rate (nombre de nom / nombre de mots) : 
+« ce taux est souvent considéré comme un indicateur pour déterminer combien ce titre est informatif »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+décide de traiter les partitions séparément et ramènent celles-ci à deux titres indépendants, l’un étant le titre, l’autre le sous-titre. 
+Hard sciences / soft sciences
+hard sciences : +mots +noun phrase +substantive word rate -the au début
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Étude du « the » au début</t>
+    </r>
+  </si>
+  <si>
+    <t>Legallois, Tutin</t>
+  </si>
+  <si>
+    <t>MR13</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sinclair, J. (1991). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Corpus, concordance, collocation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Oxford University Press.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Développe la notion de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>collocation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dans le cadre de la linguistique de corpus = expressions récurrentes
+vs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colligations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> qui renvoient principalement à l'environnement grammatical privilégié du mot (Legallois 2012b)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Principe phraséologique de la langue, le idiom principle, selon lequel les locuteurs sélectionneraient des pans de la langue préconstruits, intégrant à la fois lexique et grammaire (traduit par Legallois, Tutin, 2013).</t>
+    </r>
+  </si>
+  <si>
+    <t>Hoey</t>
+  </si>
+  <si>
+    <t>Biber</t>
+  </si>
+  <si>
+    <t>Extrait des paquets lexicaux / lexical bundles spécifiques des discours scientifiques,
+afin de caractériser au plus près le genre.</t>
+  </si>
+  <si>
+    <t>Le web n'est pas un corpus : il évolue et n'est pas clos !
+Extended lexical unit (repris par Legallois, Tutin, 2013) :
+unité lexical étendue.
+4 critères de définition : collocation, colligation, préférence sémantique, prosodie sémantique
+ex : histoire de +V dans Legallois 2012a</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Décrit le livre introuvable de Hunston &amp; Francis (pattern grammar, contextualiste) :
 Ils définissent un truc aussi générique que V n
 Corpus data &gt; introspection (c'est du driven car peu présupposés théoriques)
@@ -2053,12 +2315,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>La distinction lexique / grammaire s'efface car les lexèmes s'inscrivent dans des patterns grammaticaux</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Comparaison de [Grammaire de construction &lt;- L cognitive ] vs 
+      <t>La distinction lexique / grammaire s'efface car les lexèmes s'inscrivent dans des patterns grammaticaux
+Legallois, Tutin, 2013 en parle aussi : patron = uine configuration syntaxique, la dimension du patorn est indépendante de la notion de syntagme.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Comparaison de [Grammaire de construction &lt;- L cognitive (Fillmore) ] vs 
   [Grammaire de patrons/patrons](association fréquente entre un mot cible +d'autres mots)
  </t>
     </r>
@@ -2116,6 +2379,26 @@
     </r>
   </si>
   <si>
+    <t>Fillmore</t>
+  </si>
+  <si>
+    <t>De Legallois, Tutin, 2013 : les constructions "possèdent des propriétés grammaticales, sémantiques
+et pragamatiques qui ne sont pas prédictibles à partir de leurs parties." "ces constructions sont signifiantes en partie indépendamment du lexique qu'elles intègrent."</t>
+  </si>
+  <si>
+    <t>1988
+1999</t>
+  </si>
+  <si>
+    <t>Fillmore C. (1988) "The mechanismes of construction grammar", Berkeley Linguistics Society 14, 35-55.</t>
+  </si>
+  <si>
+    <t>Bybee</t>
+  </si>
+  <si>
+    <t>Language, Usage and Cognition, Cambridge: Cambridge University Press</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -2125,117 +2408,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>paradoxe de l'observateur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : celui-ci souhaite observer ce qui se passe quand il n’est pas là.
-Mais finalement, celui-ci postule qu'il y a une situation SANS modification, "PURE", dans une perspective positiviste… = "une réalité neutre, indépendante de la perspective prise par l'observateur"
-Astuce pour contourner le paradoxe. Mais attention à aller "trop loin" (espionnage) : interview, groupe de parole...
-Labov (82) et Milroy (87) =&gt; deux grands noms de l'enquête sociolinguistique
-Cameron Deborah (1992-1993) va très loin : il faut, outre une démarche Éthique (sur eux), défendre (pour eux) et même empowerer (avec eux) les personnes de notre sujet d'étude.
-Ex : auto-commentaire des interrogés sur leur discours
-! différence entre ceux que l'on sait et ce que l'on fait dans ces questions...
-Dans tous les cas, le sujet de notre étude, ce sont des personnes avec la considération éthique, politique et sociale nécessaire.
+      <t>amorçage lexical / lexical priming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : (pousse plus loin le principe phraséologique de la langue initié par Sinclair, 1991)
+par Legallois, Tutin, 2013 :
+"l'emploi d'un mot est en quelque sorte déterminé ("amorcé") par les emplois co-textuels et contextuels antérieurs dans lesquels il apparaît, qu'il s'agisse de l'environnement lexical et des collocations, mais aussi de son environnement sémantique, syntaxique (avec les "colligations"), pragmatique et discursif."
+par Legallois, 2006 :
+"un lexème est acquis grâce à ses occurrences dans les discours et textes, il se charge cumulativement des contextes et des co-textes dans lesquels il est "rencontré".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phraséologie = étude des séquences lexicales perçues comme préconstruites</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Élargie son sujet d'étude : principe phraséologique du langage tout entier.
+Ses objets d'études s'émancipent de la lexicologie mais leurs contours deviennent + flous
+Continuum des associations passagères aux expressions figées=unités indécomposables. 
+Avec au milieu des "séries phraséologiques" = collocations récurrentes/affinités
 </t>
     </r>
-  </si>
-  <si>
-    <t>Townsend</t>
-  </si>
-  <si>
-    <t>Reprend Dillon (1981) qui mettait en relation la présence d'un colon avec la publication :
-il comparait 474 titres non publiés vs 314 titres publiés
-Townsend fait de même avec des journaux néo-zélandais :
-OK, pour le rapport publié / non publié
-Par contre, faible relation avec l'impact mesuré par nombre de citations.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Townsend, M. A. (1983). Titular Colonicity and Scholarship: New Zealand Research and Scholarly Impact. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Zealand Journal of Psychology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 41-43.</t>
-    </r>
-  </si>
-  <si>
-    <t>« En raison de sa finitude, le corpus ne réalise donc qu'une part infime de ce qui est réalisable. (…)
-Et en toute rigueur, une grammaire construite à partir d'un corpus ne vaut que pour le corpus qui l'a produite. »</t>
-  </si>
-  <si>
-    <t>3 dicho : langue/parole=prodlang, signifiant/signifié=concept mental, diachro/synchro
-chapitre IV pour la définition de la dicho lang/parole
-&gt; ne pas oublier de rajouter le "référant", venu + tard, la chose du monde, à signifiant/signifié.</t>
-  </si>
-  <si>
-    <t>Nagano</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nagano, R. L. (2015). Research article titles and disciplinary conventions: A corpus study of eight disciplines. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Journal of Academic Writing, 5(1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 133-144.</t>
-    </r>
-  </si>
-  <si>
-    <t>MR12</t>
-  </si>
-  <si>
-    <t>MR11</t>
-  </si>
-  <si>
-    <t>MR10</t>
-  </si>
-  <si>
-    <t>MR9</t>
-  </si>
-  <si>
-    <t>MR8</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2245,8 +2461,140 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Substantive word rate (nombre de nom / nombre de mots) : 
-« ce taux est souvent considéré comme un indicateur pour déterminer combien ce titre est informatif »</t>
+      <t xml:space="preserve">Critère : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"le</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> figement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> est affaire de continuum":
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> non -compositionnalité sémantique (sens de A+B != sens de A + sens B
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> non actualisation des référents : accorder ses violons : il n'y a pas de violons accessibles
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fixité syntaxique </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> restriction combinatoire (avec synonymes ou co-hyponymes)
+Historique : Bréal (1987) avant Bally (1909)
+L'apprenant peut se tromper, employant un quasi-synonyme mais qui sonne pas bien.
+Problème de traduction aussi : de rien, you're welcome.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mais parfois rapprochement : 7 ciel en fr, en, d. "existence de ces expressions est motivée par des métaphores productives et en partie universelles" (Kövesces 2000)</t>
     </r>
     <r>
       <rPr>
@@ -2257,9 +2605,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-décide de traiter les partitions séparément et ramènent celles-ci à deux titres indépendants, l’un étant le titre, l’autre le sous-titre. 
-Hard sciences / soft sciences
-hard sciences : +mots +noun phrase +substantive word rate -the au début
+Remise en cause de la séparation lexique / grammaire au profit d'un lien étroit car le choix du lexique "impose" une construction syntaxique.
+Gross 1982 : caractère préconstruit de la majorité des phrases
 </t>
     </r>
     <r>
@@ -2271,8 +2618,108 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Étude du « the » au début</t>
-    </r>
+      <t>outils informatiques =&gt; méthodes lexicométriques capables d'ientifier les segments répétés (Salem, 1987) &lt;= le 1er il semble</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Pour s'affranchir de l'ordre linéaire </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"contrainte qui constitue une limite des approches classiques par segments répétées" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Tutin 2010) =&gt; on passe à la notion de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>motif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+"collocstruction" dans le cadre de la grammaire constructive par Stefabiwitsch et Gries 2003
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Synthèse de l'apport de la psycholinguistique à la phraséologie : Wray 2002
+Différents endroits du cerveau enregistre différentes productions linguistiques
+certaines sont enregistrées avec des slots de liberté = grammaire (comme compétence pyshcolinguistique) = "a pour origine un répertoire d'unités phraséologiques contextuellement situées" =&gt; on rejoint Sinclair). Mais  « déformabilité des unités mémorisées pour générer des énoncés nouveaux » =&gt; sinon on est condamné à répéter only.
+Une fonction principale = promotion de l'intérêt personnel du locuteur, "avantage cognitif que confèrent les unités phraséologiques mémorisées et donc rapidement disponibles et facilement énonçables" (et donc facilement récevable)</t>
+    </r>
+  </si>
+  <si>
+    <t>Longrée, D., &amp; Mellet, S.</t>
+  </si>
+  <si>
+    <r>
+      <t>Longrée, D., &amp; Mellet, S. (2013). Le motif: une unité phraséologique englobante? Étendre le champ de la phraséologie de la langue au discours. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Langages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, (1), 65-79.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cité par Legallois &amp; Tutin 2013 : présente le motif comme unité phraséologique pour ce défaire de
+la limite de l'ordre qui colle aux patrons.</t>
   </si>
 </sst>
 </file>
@@ -2462,7 +2909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2569,6 +3016,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2891,11 +3347,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7BB45F-7C76-4B6C-9D19-22CA475005CE}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,1270 +3370,1392 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="9">
         <v>2014</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H2" s="19">
         <v>10</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="7">
         <v>2003</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H3" s="6">
         <v>25</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="7">
         <v>2002</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="6">
         <v>9</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="8">
-        <v>1998</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" s="6">
-        <v>223</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>156</v>
-      </c>
+      <c r="C5" s="7">
+        <v>2006</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
+        <v>1998</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="6">
+        <v>223</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="9">
         <v>2017</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="D7" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="6">
         <v>377</v>
       </c>
-      <c r="I6" s="33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H7" s="6">
-        <v>18</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I7" s="33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>43</v>
+        <v>2002</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="H8" s="6">
-        <v>15</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>158</v>
+        <v>18</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="B9" s="16"/>
-      <c r="C9" s="8">
-        <v>1990</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H9" s="6">
-        <v>179</v>
-      </c>
+      <c r="C9" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="I9" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="7">
+        <v>2008</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="6">
+        <v>15</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="8">
+        <v>1990</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="6">
+        <v>179</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="7">
         <v>2004</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="6">
         <v>23</v>
       </c>
-      <c r="I10" s="34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="9">
+      <c r="I12" s="34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="9">
         <v>2012</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="D13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="7" t="s">
+      <c r="D14" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="H12" s="37">
+      <c r="F14" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="H14" s="37">
         <v>12046</v>
       </c>
-      <c r="I12" s="34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H13" s="6">
-        <v>105</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="8">
-        <v>1998</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14" s="6">
-        <v>61</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>196</v>
+      <c r="I14" s="34" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="7">
-        <v>2005</v>
+        <v>2003</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="H15" s="6">
-        <v>5</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>211</v>
+        <v>195</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="8">
+        <v>1998</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>196</v>
       </c>
       <c r="H16" s="6">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="I16" s="33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>206</v>
+        <v>231</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>233</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="6">
-        <v>170</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>164</v>
+        <v>232</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="B18" s="16"/>
-      <c r="C18" s="8">
-        <v>1994</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
+      <c r="C18" s="7">
+        <v>2005</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="8">
-        <v>1997</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>43</v>
+        <v>134</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2003</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>135</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>207</v>
       </c>
       <c r="H19" s="6">
-        <v>504</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>83</v>
+        <v>2009</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>119</v>
+        <v>204</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>148</v>
       </c>
       <c r="H20" s="6">
-        <v>160</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>166</v>
+        <v>170</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="8">
-        <v>1972</v>
+        <v>1994</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="B22" s="16"/>
-      <c r="C22" s="9">
-        <v>2011</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="C22" s="8">
+        <v>1997</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" s="6">
+        <v>504</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="B23" s="16"/>
       <c r="C23" s="7">
-        <v>2001</v>
+        <v>2004</v>
       </c>
       <c r="D23" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>209</v>
+      <c r="G23" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="H23" s="6">
-        <v>22</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>207</v>
+        <v>160</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" s="16"/>
-      <c r="C24" s="7">
-        <v>2002</v>
+      <c r="C24" s="8">
+        <v>1972</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>32</v>
+        <v>2005</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="40" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B26" s="16"/>
-      <c r="C26" s="7">
+      <c r="C26" s="9">
+        <v>2011</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="7">
         <v>2001</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H26" s="6">
-        <v>23</v>
-      </c>
-      <c r="I26" s="33" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="7">
-        <v>2000</v>
-      </c>
       <c r="D27" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>195</v>
+        <v>202</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>229</v>
       </c>
       <c r="H27" s="6">
+        <v>22</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="7">
+        <v>2002</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="C28" s="7">
-        <v>2006</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="H28" s="6">
-        <v>54</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>203</v>
+      <c r="I28" s="32" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="7">
-        <v>2006</v>
+        <v>2002</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="H29" s="6">
-        <v>21</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>169</v>
+        <v>89</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>34</v>
+        <v>2001</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H30" s="6">
-        <v>24</v>
-      </c>
-      <c r="I30" s="34" t="s">
-        <v>170</v>
+        <v>23</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="7">
-        <v>2005</v>
+        <v>2000</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>206</v>
+        <v>82</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>193</v>
       </c>
       <c r="H31" s="6">
-        <v>83</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="8">
-        <v>1988</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>33</v>
+        <v>203</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" s="7">
+        <v>2006</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I32" s="32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="H32" s="6">
+        <v>54</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>74</v>
+        <v>221</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2013</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>199</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>34</v>
+        <v>2006</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I34" s="32" t="s">
-        <v>3</v>
+        <v>204</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H34" s="6">
+        <v>21</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="7">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H35" s="6">
-        <v>488</v>
+        <v>24</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B36" s="16"/>
-      <c r="C36" s="8">
-        <v>1977</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>43</v>
+      <c r="C36" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="H36" s="6">
-        <v>304</v>
-      </c>
-      <c r="I36" s="34" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>219</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="B37" s="16"/>
       <c r="C37" s="9">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F37" s="35" t="s">
-        <v>206</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="F37" s="6"/>
       <c r="G37" s="28" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="H37" s="6">
-        <v>9</v>
-      </c>
-      <c r="I37" s="29" t="s">
-        <v>218</v>
+        <v>51</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="B38" s="16"/>
-      <c r="C38" s="9">
-        <v>2010</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>43</v>
+      <c r="C38" s="8">
+        <v>1988</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>33</v>
+        <v>2002</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>30</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B40" s="16"/>
-      <c r="C40" s="9" t="s">
-        <v>51</v>
+      <c r="C40" s="7">
+        <v>2005</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="H40" s="6">
-        <v>236</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>174</v>
+        <v>204</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B41" s="16"/>
-      <c r="C41" s="9">
-        <v>2017</v>
+      <c r="C41" s="7">
+        <v>2005</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>53</v>
+        <v>204</v>
       </c>
       <c r="H41" s="6">
-        <v>4</v>
+        <v>488</v>
       </c>
       <c r="I41" s="34" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B42" s="16"/>
-      <c r="C42" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>75</v>
+      <c r="C42" s="8">
+        <v>1977</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F42" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>134</v>
+        <v>204</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="H42" s="6">
-        <v>207</v>
+        <v>304</v>
       </c>
       <c r="I42" s="34" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="7">
-        <v>2009</v>
+        <v>213</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" s="9">
+        <v>2015</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>83</v>
+        <v>202</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>220</v>
       </c>
       <c r="H43" s="6">
-        <v>17</v>
-      </c>
-      <c r="I43" s="33" t="s">
-        <v>177</v>
+        <v>9</v>
+      </c>
+      <c r="I43" s="29" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="9">
         <v>2010</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="H44" s="6">
-        <v>176</v>
-      </c>
-      <c r="I44" s="33" t="s">
-        <v>190</v>
+        <v>82</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="7">
+        <v>2003</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I45" s="32" t="s">
         <v>29</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="6">
-        <v>3367</v>
-      </c>
-      <c r="I45" s="33" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="9">
-        <v>2015</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>93</v>
+      <c r="C46" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>204</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="H46" s="6">
-        <v>3</v>
-      </c>
-      <c r="I46" s="33" t="s">
-        <v>178</v>
+        <v>236</v>
+      </c>
+      <c r="I46" s="34" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="8">
-        <v>1991</v>
+      <c r="C47" s="9">
+        <v>2017</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I47" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B48" s="16"/>
       <c r="C48" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D48" s="17" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>74</v>
       </c>
       <c r="F48" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G48" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H48" s="37">
-        <v>1426</v>
-      </c>
-      <c r="I48" s="32" t="s">
-        <v>152</v>
+        <v>204</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="6">
+        <v>207</v>
+      </c>
+      <c r="I48" s="34" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="9">
-        <v>2015</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>116</v>
+      <c r="A49" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="16"/>
+      <c r="C49" s="7">
+        <v>2009</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>204</v>
       </c>
       <c r="H49" s="6">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="I49" s="33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>26</v>
+        <v>189</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I50" s="32" t="s">
-        <v>5</v>
+      <c r="C50" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="H50" s="6">
+        <v>176</v>
+      </c>
+      <c r="I50" s="33" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="8">
-        <v>1996</v>
+      <c r="C51" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F51" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H51" s="37">
-        <v>2055</v>
-      </c>
-      <c r="I51" s="32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51" s="6">
+        <v>3367</v>
+      </c>
+      <c r="I51" s="33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C52" s="8">
-        <v>1983</v>
-      </c>
-      <c r="D52" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H52" s="6">
+        <v>3</v>
+      </c>
+      <c r="I52" s="33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="16"/>
+      <c r="C53" s="8">
+        <v>1991</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="F52" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="H52" s="6">
-        <v>10</v>
-      </c>
-      <c r="I52" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="9">
-        <v>2013</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F53" s="35" t="s">
-        <v>206</v>
+      <c r="G53" s="28" t="s">
+        <v>224</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="7">
         <v>2004</v>
       </c>
-      <c r="D54" s="21" t="s">
-        <v>83</v>
+      <c r="D54" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F54" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="H54" s="6">
-        <v>16</v>
-      </c>
-      <c r="I54" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="I55" s="32" t="s">
-        <v>73</v>
+        <v>204</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="H54" s="37">
+        <v>1426</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H55" s="6">
+        <v>68</v>
+      </c>
+      <c r="I55" s="33" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B56" s="16"/>
-      <c r="C56" s="9">
+      <c r="C56" s="7">
+        <v>2009</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I56" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="8">
+        <v>1996</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H57" s="37">
+        <v>2055</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1983</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G58" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H58" s="6">
+        <v>10</v>
+      </c>
+      <c r="I58" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="9">
+        <v>2013</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="16"/>
+      <c r="C60" s="7">
+        <v>2004</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H60" s="6">
+        <v>16</v>
+      </c>
+      <c r="I60" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="16"/>
+      <c r="C61" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G61" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="I61" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="9">
         <v>2012</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D62" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G62" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F56" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="G56" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H56" s="6">
+      <c r="H62" s="6">
         <v>0</v>
       </c>
-      <c r="I56" s="34" t="s">
-        <v>181</v>
+      <c r="I62" s="34" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4205,113 +4783,113 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>2001</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>2001</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>2000</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <v>1991</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4346,101 +4924,101 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
         <v>96</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
         <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
         <v>106</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
         <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4463,18 +5041,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4497,43 +5075,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dossier : sur les résultats. 9 TODO
</commit_message>
<xml_diff>
--- a/dossiers/Final - Références articles.xlsx
+++ b/dossiers/Final - Références articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BF6E62-837D-4210-800B-93962B4E2AA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB38A1D-8D47-434B-A245-85CBE55694A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="246">
   <si>
     <t>Gross, M. (1994). Dictionnaires électroniques et traduction automatique. Langages, 48-58.</t>
   </si>
@@ -2720,6 +2720,47 @@
   <si>
     <t>Cité par Legallois &amp; Tutin 2013 : présente le motif comme unité phraséologique pour ce défaire de
 la limite de l'ordre qui colle aux patrons.</t>
+  </si>
+  <si>
+    <t>Jacques &amp; Sebire</t>
+  </si>
+  <si>
+    <t>Ils précisent que plus le titre sera long, plus il sera susceptible de contenir des mots de requêtes et donc d’être associer à ces requêtes les contenant pour être ensuite trouvé
+Ils montrent que les 25 titres les plus cités dans 3 journaux médicaux « ont plus de deux fois plus de mots dans le titre que les articles les moins cités »
+Ils sont de l'avis que « beaucoup de chercheurs peuvent plus fréquemment connaître ou utiliser l’acronyme plutôt que le nom complet »
+Concerne les lexèmes du titre et plus particulièrement la présence d’un nom de pays. Du fait de sa présence, il précise son objet d’étude en le limitant, ce qui contribue au fait qu’il soit moins cité du fait de sa spécialisation.
+En ce qui concerne la présence d’un double point ou l’augmentation de la longueur et le nombre de citations : si y'en a un, si c + long : + de citations
+Citent sans les reprendre d’autres caractéristiques comme le genre des auteurs qui influe sur sa probabilité d’acceptation dans une revue ou son nombre futur de citations selon (Ayres, 2008).
+300 titres, 150 les + cités, 150 les - cités, tirés de 3 journaux à travers Web of Science</t>
+  </si>
+  <si>
+    <t>MR14</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jacques, T. S., &amp; Sebire, N. J. (2010). The impact of article titles on citation hits: an analysis of general and specialist medical journals. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Journal of the Royal Society of Medicine Short Reports</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 1-5.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3347,11 +3388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7BB45F-7C76-4B6C-9D19-22CA475005CE}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,66 +3965,74 @@
         <v>237</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="16"/>
+        <v>242</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>244</v>
+      </c>
       <c r="C26" s="9">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>82</v>
+        <v>202</v>
       </c>
       <c r="F26" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="I26" s="33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="G26" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="H26" s="6">
+        <v>117</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2001</v>
+        <v>84</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="9">
+        <v>2011</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>202</v>
+        <v>82</v>
       </c>
       <c r="F27" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G27" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="H27" s="6">
-        <v>22</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="16"/>
+        <v>206</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="C28" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
+        <v>2001</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="F28" s="35" t="s">
         <v>204</v>
       </c>
+      <c r="G28" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H28" s="6">
+        <v>22</v>
+      </c>
       <c r="I28" s="32" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3994,259 +4043,259 @@
       <c r="C29" s="7">
         <v>2002</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>32</v>
+      <c r="D29" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F29" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G29" s="27" t="s">
-        <v>89</v>
-      </c>
       <c r="I29" s="32" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>73</v>
+        <v>2002</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F30" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="H30" s="6">
-        <v>23</v>
-      </c>
-      <c r="I30" s="33" t="s">
-        <v>166</v>
+      <c r="G30" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="7">
+        <v>2001</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H31" s="6">
+        <v>23</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="7">
         <v>2000</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F32" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="G32" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H32" s="6">
         <v>204</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+    <row r="33" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B33" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C33" s="7">
         <v>2006</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="H32" s="6">
-        <v>54</v>
-      </c>
-      <c r="I32" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C33" s="9">
-        <v>2013</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="F33" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G33" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="I33" s="29"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="H33" s="6">
+        <v>54</v>
+      </c>
+      <c r="I33" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="7">
-        <v>2006</v>
+        <v>221</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="9">
+        <v>2013</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F34" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G34" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="H34" s="6">
-        <v>21</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>167</v>
-      </c>
+      <c r="G34" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="7">
-        <v>2008</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>33</v>
+        <v>2006</v>
       </c>
       <c r="F35" s="35" t="s">
         <v>204</v>
       </c>
+      <c r="G35" s="27" t="s">
+        <v>142</v>
+      </c>
       <c r="H35" s="6">
-        <v>24</v>
-      </c>
-      <c r="I35" s="34" t="s">
-        <v>168</v>
+        <v>21</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>82</v>
+        <v>2008</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F36" s="35" t="s">
         <v>204</v>
       </c>
       <c r="H36" s="6">
+        <v>24</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="6">
         <v>83</v>
       </c>
-      <c r="I36" s="33" t="s">
+      <c r="I37" s="33" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+    <row r="38" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="9">
+      <c r="B38" s="16"/>
+      <c r="C38" s="9">
         <v>2013</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="28" t="s">
+      <c r="F38" s="6"/>
+      <c r="G38" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H38" s="6">
         <v>51</v>
       </c>
-      <c r="I37" s="33" t="s">
+      <c r="I38" s="33" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="8">
+      <c r="B39" s="16"/>
+      <c r="C39" s="8">
         <v>1988</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="I38" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="7">
-        <v>2002</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>73</v>
       </c>
       <c r="F39" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G39" s="23" t="s">
-        <v>211</v>
-      </c>
       <c r="I39" s="32" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>33</v>
+        <v>2002</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F40" s="35" t="s">
         <v>204</v>
       </c>
+      <c r="G40" s="23" t="s">
+        <v>211</v>
+      </c>
       <c r="I40" s="32" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="7">
@@ -4255,26 +4304,20 @@
       <c r="D41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="F41" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="H41" s="6">
-        <v>488</v>
-      </c>
-      <c r="I41" s="34" t="s">
-        <v>170</v>
+      <c r="I41" s="32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="16"/>
-      <c r="C42" s="8">
-        <v>1977</v>
+      <c r="C42" s="7">
+        <v>2005</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>33</v>
@@ -4285,124 +4328,121 @@
       <c r="F42" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G42" s="27" t="s">
-        <v>66</v>
-      </c>
       <c r="H42" s="6">
-        <v>304</v>
+        <v>488</v>
       </c>
       <c r="I42" s="34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C43" s="9">
-        <v>2015</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>202</v>
+        <v>18</v>
+      </c>
+      <c r="B43" s="16"/>
+      <c r="C43" s="8">
+        <v>1977</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F43" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G43" s="28" t="s">
-        <v>220</v>
+      <c r="G43" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="H43" s="6">
-        <v>9</v>
-      </c>
-      <c r="I43" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="I43" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="16"/>
+        <v>213</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>215</v>
+      </c>
       <c r="C44" s="9">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="F44" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G44" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>183</v>
+      <c r="G44" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="H44" s="6">
+        <v>9</v>
+      </c>
+      <c r="I44" s="29" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>19</v>
+        <v>186</v>
       </c>
       <c r="B45" s="16"/>
-      <c r="C45" s="7">
-        <v>2003</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>32</v>
+      <c r="C45" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F45" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="I45" s="32" t="s">
-        <v>29</v>
+      <c r="G45" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>42</v>
+      <c r="C46" s="7">
+        <v>2003</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F46" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G46" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="H46" s="6">
-        <v>236</v>
-      </c>
-      <c r="I46" s="34" t="s">
-        <v>172</v>
+      <c r="I46" s="32" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="9">
-        <v>2017</v>
+      <c r="C47" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>42</v>
@@ -4411,229 +4451,238 @@
         <v>204</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H47" s="6">
-        <v>4</v>
+        <v>236</v>
       </c>
       <c r="I47" s="34" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>74</v>
+      <c r="C48" s="9">
+        <v>2017</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F48" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G48" s="28" t="s">
-        <v>132</v>
+      <c r="G48" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="H48" s="6">
-        <v>207</v>
+        <v>4</v>
       </c>
       <c r="I48" s="34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B49" s="16"/>
       <c r="C49" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>82</v>
+        <v>2005</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="F49" s="35" t="s">
         <v>204</v>
       </c>
+      <c r="G49" s="28" t="s">
+        <v>132</v>
+      </c>
       <c r="H49" s="6">
-        <v>17</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>175</v>
+        <v>207</v>
+      </c>
+      <c r="I49" s="34" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="9">
-        <v>2010</v>
+      <c r="C50" s="7">
+        <v>2009</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F50" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="G50" s="27" t="s">
-        <v>190</v>
+      <c r="F50" s="35" t="s">
+        <v>204</v>
       </c>
       <c r="H50" s="6">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="I50" s="33" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>20</v>
+        <v>189</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>33</v>
+      <c r="C51" s="9">
+        <v>2010</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>92</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="H51" s="6">
-        <v>3367</v>
+        <v>176</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="9">
-        <v>2015</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>39</v>
+      <c r="C52" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>92</v>
       </c>
       <c r="G52" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H52" s="6">
+        <v>3367</v>
+      </c>
+      <c r="I52" s="33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="16"/>
+      <c r="C53" s="9">
+        <v>2015</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H53" s="6">
         <v>3</v>
       </c>
-      <c r="I52" s="33" t="s">
+      <c r="I53" s="33" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="8">
-        <v>1991</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F53" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>73</v>
+      <c r="C54" s="8">
+        <v>1991</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F54" s="35" t="s">
         <v>204</v>
       </c>
       <c r="G54" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="I54" s="32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="7">
+        <v>2004</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G55" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="H54" s="37">
+      <c r="H55" s="37">
         <v>1426</v>
       </c>
-      <c r="I54" s="32" t="s">
+      <c r="I55" s="32" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="9">
+      <c r="B56" s="13"/>
+      <c r="C56" s="9">
         <v>2015</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D56" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G55" s="27" t="s">
+      <c r="G56" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H56" s="6">
         <v>68</v>
       </c>
-      <c r="I55" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="7">
-        <v>2009</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F56" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="I56" s="32" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B57" s="16"/>
-      <c r="C57" s="8">
-        <v>1996</v>
+      <c r="C57" s="7">
+        <v>2009</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>33</v>
@@ -4641,120 +4690,138 @@
       <c r="F57" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="H57" s="37">
-        <v>2055</v>
-      </c>
       <c r="I57" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>216</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B58" s="16"/>
       <c r="C58" s="8">
-        <v>1983</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>202</v>
+        <v>1996</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F58" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G58" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="H58" s="6">
-        <v>10</v>
-      </c>
-      <c r="I58" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="37">
+        <v>2055</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="9">
-        <v>2013</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>33</v>
+        <v>208</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1983</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="F59" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="I59" s="32" t="s">
-        <v>6</v>
+      <c r="G59" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H59" s="6">
+        <v>10</v>
+      </c>
+      <c r="I59" s="29" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="7">
-        <v>2004</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>82</v>
+      <c r="C60" s="9">
+        <v>2013</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="F60" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="H60" s="6">
-        <v>16</v>
-      </c>
-      <c r="I60" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="I60" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B61" s="16"/>
       <c r="C61" s="7">
-        <v>2005</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>73</v>
+        <v>2004</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="F61" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G61" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="I61" s="32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="6">
+        <v>16</v>
+      </c>
+      <c r="I61" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="9">
-        <v>2012</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>45</v>
+      <c r="C62" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="F62" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G62" s="27" t="s">
+      <c r="G62" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="16"/>
+      <c r="C63" s="9">
+        <v>2012</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="H62" s="6">
+      <c r="H63" s="6">
         <v>0</v>
       </c>
-      <c r="I62" s="34" t="s">
+      <c r="I63" s="34" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dossier : v1 :-)
</commit_message>
<xml_diff>
--- a/dossiers/Final - Références articles.xlsx
+++ b/dossiers/Final - Références articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B695CF14-E70C-4609-BEE2-5C02CB684E29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CB113-F97B-4C6E-88A7-44B34F863958}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
   </bookViews>
@@ -2775,12 +2775,114 @@
     </r>
   </si>
   <si>
+    <t>Adler Silvia</t>
+  </si>
+  <si>
+    <t>Auteurs (Last edit : 2018-08-05)</t>
+  </si>
+  <si>
+    <t>MR15</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plus de 50% des articles publiés ne sont jamais cités. Cela monte à 95% dans certaines disciplines !</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ils précisent que plus le titre sera long, plus il sera susceptible de contenir des mots de requêtes et donc d’être associer à ces requêtes les contenant pour être ensuite trouvé
+Ils montrent que les 25 titres les plus cités dans 3 journaux médicaux « ont plus de deux fois plus de mots dans le titre que les articles les moins cités »
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ils sont de l'avis que « beaucoup de chercheurs peuvent plus fréquemment connaître ou utiliser l’acronyme plutôt que le nom complet »</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Concerne les lexèmes du titre et plus particulièrement la présence d’un nom de pays. Du fait de sa présence, il précise son objet d’étude en le limitant, ce qui contribue au fait qu’il soit moins cité du fait de sa spécialisation.
+En ce qui concerne la présence d’un double point ou l’augmentation de la longueur et le nombre de citations : si y'en a un, si c + long : + de citations
+Citent sans les reprendre d’autres caractéristiques comme le genre des auteurs qui influe sur sa probabilité d’acceptation dans une revue ou son nombre futur de citations selon (Ayres, 2008).
+300 titres, 150 les + cités, 150 les - cités, tirés de 3 journaux à travers Web of Science</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">noms généraux sous-spécifiés au sein d'une sémantique discursive
-NSS se spécifie grâce au contexte (très souvent détermination démonstrative par ex : ce/cet/cette : "impose un point de vue nouveau sur l'entitée représentée par lui mais aussi annule en même temps d'autres significiations")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NSS se spécifie grâce au contexte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (très souvent détermination démonstrative par ex : ce/cet/cette : "impose un point de vue nouveau sur l'entitée représentée par lui mais aussi annule en même temps d'autres significiations")
 À "besoin d'un contexte pour s'imprégner lexicalement". Pour Hunston &amp; Francis (2000 : 185) ces noms exigent une "lexicalisation".
 signification lexicale insufisante (p6)
-comment faire l'interprétation référentielle ? via une connexion qui la stature
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>comment faire l'interprétation référentielle ? via une connexion qui la stature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 besoin d'autres unités relevant de rangs différents (du GN à la séquence)
 - nom général =&gt; Halliday &amp; Hasan, 1976
 - nom sous-spécifié =&gt; Legallois 2006, 2008
@@ -2980,66 +3082,6 @@
       </rPr>
       <t>construction du sens et de la signification en rapport avec les NGSS = "faire état de la tension entre stabilité (fixisme : le sens du signe dans le lexique) d'une part, et dynamicité (rapports avec les autres signes coprésents ; influence réciproque des nuités présentes) ou variabilité (convergences et divergences relatives à la variabilité paradigmatique) d'autre part".
 "le nom sous-spécifié perspectivise le contexte, mais c'est le contexte qui stabilise le nom."</t>
-    </r>
-  </si>
-  <si>
-    <t>Adler Silvia</t>
-  </si>
-  <si>
-    <t>Auteurs (Last edit : 2018-08-05)</t>
-  </si>
-  <si>
-    <t>MR15</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Plus de 50% des articles publiés ne sont jamais cités. Cela monte à 95% dans certaines disciplines !</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Ils précisent que plus le titre sera long, plus il sera susceptible de contenir des mots de requêtes et donc d’être associer à ces requêtes les contenant pour être ensuite trouvé
-Ils montrent que les 25 titres les plus cités dans 3 journaux médicaux « ont plus de deux fois plus de mots dans le titre que les articles les moins cités »
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ils sont de l'avis que « beaucoup de chercheurs peuvent plus fréquemment connaître ou utiliser l’acronyme plutôt que le nom complet »</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Concerne les lexèmes du titre et plus particulièrement la présence d’un nom de pays. Du fait de sa présence, il précise son objet d’étude en le limitant, ce qui contribue au fait qu’il soit moins cité du fait de sa spécialisation.
-En ce qui concerne la présence d’un double point ou l’augmentation de la longueur et le nombre de citations : si y'en a un, si c + long : + de citations
-Citent sans les reprendre d’autres caractéristiques comme le genre des auteurs qui influe sur sa probabilité d’acceptation dans une revue ou son nombre futur de citations selon (Ayres, 2008).
-300 titres, 150 les + cités, 150 les - cités, tirés de 3 journaux à travers Web of Science</t>
     </r>
   </si>
 </sst>
@@ -3243,7 +3285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3368,6 +3410,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3694,7 +3739,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3713,7 +3758,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="2" t="s">
@@ -3740,10 +3785,10 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" s="9">
         <v>2018</v>
@@ -3756,12 +3801,12 @@
         <v>203</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="45" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4311,7 +4356,7 @@
         <v>203</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H27" s="6">
         <v>117</v>

</xml_diff>

<commit_message>
Corrections du dossier + stats sur big corpus
</commit_message>
<xml_diff>
--- a/dossiers/Final - Références articles.xlsx
+++ b/dossiers/Final - Références articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CB113-F97B-4C6E-88A7-44B34F863958}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA71185C-F306-4FC2-BF2A-DACFB987D5EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{31378B4E-CA3D-4676-82E6-FC3F50E855D4}"/>
   </bookViews>
@@ -268,9 +268,6 @@
     <t>Dal Namer</t>
   </si>
   <si>
-    <t>Cori David</t>
-  </si>
-  <si>
     <t>Gilquin Gries</t>
   </si>
   <si>
@@ -532,65 +529,6 @@
 stockés électroniquement sous un format texte ».
 la linguistique de corpus « qui s’intéresse aux textes, aux
 textes réels » (Williams 2005 : 13).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Données d'Introspection (jugement d'acceptabilité surtout) pb :
-- sa subjectivité et son inconsistance inter et même intra-personnelle
-- On notera que la sélection de ces productions est subjective pourle corpus :
-garder la trace !!! Ainsi que des préparations effectuées !!!
-Il s’en déduit que travailler à l’aide de corpus permettrait de trouver de
-nouveaux faits (Kennedy 1998, Manning 2003) et, par là même, de récuser des
-connaissances faussement établies (Manning 2003).
-Cette critique de Abney rejoint des critiques plus anciennes qui visaient
-aussi bien l’opposition compétence/performance que l’opposition saussurienne
-langue/parole. Leech (1992 : 108) Halliday (1992 : 66)
-Rastier (2005 : 35),
-« les règles de la langue sont sans doute des normes invétérées et les perfor-
-mances de la parole ne restent évidemment pas exemptes de normativité : elles instancient et manifestent les règles de la langue et diverses normes sociolectales. Bref, la linguistique peut prendre de droit pour objet de description l’espace des normes : au lieu de les édicter, comme elle le faisait naguère en frappant d’inacceptabilité des énoncés alors même qu’ils sont attestés, elle doit les décrire et pour cela exploiter des corpus ».
-« [...] les corpus peuvent rassembler des énoncés sur lesquels l’analyste n’est pas forcément à même de porter des jugements d’acceptabilité. C’est le cas par exemple pour des corpus de langues mortes [...], pour des corpus de langues de spécialité [...] » (Habert et al. 1997 : 9).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.3 : difficultés des corpus :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-En ce sens, on peut dire que les résultats de la recherche dépendent des conditions matérielles de la constitution des corpus. [...] Quand on utilise des corpus annotés, on est dépendant également d’autres conditions matérielles, de la façon dont les corpus ont été annotés (choix des étiquettes, erreurs dans l’annotation, etc.).
-Il importe ensuite de noter que les données « réelles », « objectives », si l’on
-reprend les termes des tenants des approches sur corpus, ne sont jamais les
-données sur lesquelles travaille un linguiste utilisant des corpus. On le sait
-bien : les corpus doivent être préparés. On corrige, on sélectionne, on élimine,
-en fonction des traitements ultérieurs (voir pour des exemples les articles de
-Fradin et al., Delais, Geyken, ce numéro). Cette première phase peut même
-s’avérer complexe, car on peut avoir à résoudre des problèmes, pour lesquels on n’a pas de réponse assurée, pour lesquels le travail sur corpus doit justement apporter une réponse, etc. Parmi les précautions méthodologiques indispensables, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>un inventaire soigneux de toutes les décisions prises en amont doit être tenu. + pour reconnaître que quelque chose est une erreur on doit déjà savoir que c'est une erreur ! (l'oeuf la poule).</t>
     </r>
   </si>
   <si>
@@ -890,32 +828,6 @@
   </si>
   <si>
     <r>
-      <t>Cori, M., &amp; David, S. (2008). Les corpus fondent-ils une nouvelle linguistique?. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Langages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, (3), 111-129.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Courtois, B. (1990). Un système de dictionnaires électroniques pour les mots simples du français. </t>
     </r>
     <r>
@@ -2773,9 +2685,6 @@
       </rPr>
       <t>, 210,(2), 71-86. doi:10.3917/lang.210.0071.</t>
     </r>
-  </si>
-  <si>
-    <t>Adler Silvia</t>
   </si>
   <si>
     <t>Auteurs (Last edit : 2018-08-05)</t>
@@ -3082,6 +2991,117 @@
       </rPr>
       <t>construction du sens et de la signification en rapport avec les NGSS = "faire état de la tension entre stabilité (fixisme : le sens du signe dans le lexique) d'une part, et dynamicité (rapports avec les autres signes coprésents ; influence réciproque des nuités présentes) ou variabilité (convergences et divergences relatives à la variabilité paradigmatique) d'autre part".
 "le nom sous-spécifié perspectivise le contexte, mais c'est le contexte qui stabilise le nom."</t>
+    </r>
+  </si>
+  <si>
+    <t>Adler Silvia
+Sémantique des noms généraux sous-spécifiés et construction du sens</t>
+  </si>
+  <si>
+    <r>
+      <t>Cori, M., &amp; David, S. (2008). Les corpus fondent-ils une nouvelle linguistique? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Langages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, (3), 111-129.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cori David
+Les corpus fondent-ils une nouvelle linguistique?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Données d'Introspection (jugement d'acceptabilité surtout) pb :
+- sa subjectivité et son inconsistance inter et même intra-personnelle
+- On notera que la sélection de ces productions est subjective pourle corpus :
+garder la trace !!! Ainsi que des préparations effectuées !!!
+Il s’en déduit que travailler à l’aide de corpus permettrait de trouver de
+nouveaux faits (Kennedy 1998, Manning 2003) et, par là même, de récuser des
+connaissances faussement établies (Manning 2003).
+Cette critique de Abney rejoint des critiques plus anciennes qui visaient
+aussi bien l’opposition compétence/performance que l’opposition saussurienne
+langue/parole. Leech (1992 : 108) Halliday (1992 : 66)
+Rastier (2005 : 35),
+« les règles de la langue sont sans doute des normes invétérées et les performances de la parole ne restent évidemment pas exemptes de normativité : elles instancient et manifestent les règles de la langue et diverses normes sociolectales. Bref, la linguistique peut prendre de droit pour objet de description l’espace des normes : au lieu de les édicter, comme elle le faisait naguère en frappant d’inacceptabilité des énoncés alors même qu’ils sont attestés, elle doit les décrire et pour cela exploiter des corpus ».
+« [...] les corpus peuvent rassembler des énoncés sur lesquels l’analyste n’est pas forcément à même de porter des jugements d’acceptabilité. C’est le cas par exemple pour des corpus de langues mortes [...], pour des corpus de langues de spécialité [...] » (Habert et al. 1997 : 9).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.3 : difficultés des corpus :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+En ce sens, on peut dire que</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> les résultats de la recherche dépendent des conditions matérielles de la constitution des corpus. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[...] Quand on utilise des corpus annotés, on est dépendant également d’autres conditions matérielles, de la façon dont les corpus ont été annotés (choix des étiquettes, erreurs dans l’annotation, etc.).
+Il importe ensuite de noter que les données « réelles », « objectives », si l’on reprend les termes des tenants des approches sur corpus, ne sont jamais les
+données sur lesquelles travaille un linguiste utilisant des corpus. On le sait bien : les corpus doivent être préparés. On corrige, on sélectionne, on élimine,
+en fonction des traitements ultérieurs (voir pour des exemples les articles de Fradin et al., Delais, Geyken, ce numéro). Cette première phase peut même
+s’avérer complexe, car on peut avoir à résoudre des problèmes, pour lesquels on n’a pas de réponse assurée, pour lesquels le travail sur corpus doit justement apporter une réponse, etc. Parmi les précautions méthodologiques indispensables, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>un inventaire soigneux de toutes les décisions prises en amont doit être tenu. 
++ pour reconnaître que quelque chose est une erreur on doit déjà savoir que c'est une erreur ! (l'oeuf la poule).</t>
     </r>
   </si>
 </sst>
@@ -3285,7 +3305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3413,6 +3433,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3738,8 +3764,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3758,7 +3784,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="2" t="s">
@@ -3771,7 +3797,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>35</v>
@@ -3784,55 +3810,55 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>245</v>
+      <c r="A2" s="46" t="s">
+        <v>246</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C2" s="9">
         <v>2018</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="9">
         <v>2014</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H3" s="19">
         <v>10</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3847,18 +3873,18 @@
         <v>33</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H4" s="6">
         <v>25</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="7">
@@ -3868,41 +3894,41 @@
         <v>32</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="6">
         <v>9</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="7">
         <v>2006</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="28" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="8">
@@ -3912,40 +3938,40 @@
         <v>39</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H7" s="6">
         <v>223</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="9">
         <v>2017</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" s="6">
         <v>377</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3960,18 +3986,18 @@
         <v>33</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H9" s="6">
         <v>18</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="9">
@@ -3983,12 +4009,12 @@
       </c>
       <c r="F10" s="6"/>
       <c r="I10" s="34" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>79</v>
+      <c r="A11" s="47" t="s">
+        <v>248</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="7">
@@ -4001,16 +4027,16 @@
         <v>42</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>136</v>
+        <v>249</v>
       </c>
       <c r="H11" s="6">
         <v>15</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>155</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4025,13 +4051,13 @@
         <v>33</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H12" s="6">
         <v>179</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4046,13 +4072,13 @@
         <v>33</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H13" s="6">
         <v>23</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4067,13 +4093,13 @@
         <v>73</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4091,16 +4117,16 @@
         <v>42</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H15" s="37">
         <v>12046</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4115,103 +4141,103 @@
         <v>33</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H16" s="6">
         <v>105</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="8">
         <v>1998</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H17" s="6">
         <v>61</v>
       </c>
       <c r="I17" s="33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="I18" s="32" t="s">
         <v>230</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="7">
         <v>2005</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H19" s="6">
         <v>5</v>
       </c>
       <c r="I19" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C20" s="7">
         <v>2003</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="36" t="s">
         <v>203</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>206</v>
       </c>
       <c r="H20" s="6">
         <v>49</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="7">
@@ -4224,16 +4250,16 @@
         <v>42</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H21" s="6">
         <v>170</v>
       </c>
       <c r="I21" s="34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4248,7 +4274,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I22" s="32" t="s">
         <v>0</v>
@@ -4269,37 +4295,37 @@
         <v>42</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H23" s="6">
         <v>504</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="7">
         <v>2004</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H24" s="6">
         <v>160</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -4314,7 +4340,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I25" s="32" t="s">
         <v>1</v>
@@ -4322,91 +4348,91 @@
     </row>
     <row r="26" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="7">
         <v>2005</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="40" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C27" s="9">
         <v>2010</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H27" s="6">
         <v>117</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="9">
         <v>2011</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C29" s="7">
         <v>2001</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H29" s="6">
         <v>22</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4421,7 +4447,7 @@
         <v>33</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I30" s="32" t="s">
         <v>2</v>
@@ -4439,10 +4465,10 @@
         <v>32</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I31" s="32" t="s">
         <v>31</v>
@@ -4460,108 +4486,108 @@
         <v>73</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H32" s="6">
         <v>23</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="7">
         <v>2000</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H33" s="6">
         <v>204</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C34" s="7">
         <v>2006</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H34" s="6">
         <v>54</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C35" s="9">
         <v>2013</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I35" s="29"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="7">
         <v>2006</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H36" s="6">
         <v>21</v>
       </c>
       <c r="I36" s="33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4576,61 +4602,61 @@
         <v>33</v>
       </c>
       <c r="F37" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H37" s="6">
         <v>24</v>
       </c>
       <c r="I37" s="34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="7">
         <v>2005</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H38" s="6">
         <v>83</v>
       </c>
       <c r="I38" s="33" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="9">
         <v>2013</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="28" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H39" s="6">
         <v>51</v>
       </c>
       <c r="I39" s="33" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="8">
@@ -4640,7 +4666,7 @@
         <v>32</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I40" s="32" t="s">
         <v>30</v>
@@ -4658,13 +4684,13 @@
         <v>73</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4679,7 +4705,7 @@
         <v>33</v>
       </c>
       <c r="F42" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I42" s="32" t="s">
         <v>3</v>
@@ -4700,13 +4726,13 @@
         <v>42</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H43" s="6">
         <v>488</v>
       </c>
       <c r="I43" s="34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4724,7 +4750,7 @@
         <v>42</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G44" s="27" t="s">
         <v>66</v>
@@ -4733,60 +4759,60 @@
         <v>304</v>
       </c>
       <c r="I44" s="34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C45" s="9">
         <v>2015</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F45" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H45" s="6">
         <v>9</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B46" s="16"/>
       <c r="C46" s="9">
         <v>2010</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4801,7 +4827,7 @@
         <v>32</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I47" s="32" t="s">
         <v>29</v>
@@ -4822,7 +4848,7 @@
         <v>42</v>
       </c>
       <c r="F48" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G48" s="27" t="s">
         <v>51</v>
@@ -4831,7 +4857,7 @@
         <v>236</v>
       </c>
       <c r="I48" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4849,7 +4875,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G49" s="27" t="s">
         <v>52</v>
@@ -4858,7 +4884,7 @@
         <v>4</v>
       </c>
       <c r="I49" s="34" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4873,61 +4899,61 @@
         <v>74</v>
       </c>
       <c r="F50" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G50" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H50" s="6">
         <v>207</v>
       </c>
       <c r="I50" s="34" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="7">
         <v>2009</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H51" s="6">
         <v>17</v>
       </c>
       <c r="I51" s="33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="9">
         <v>2010</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H52" s="6">
         <v>176</v>
       </c>
       <c r="I52" s="33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4942,21 +4968,21 @@
         <v>33</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H53" s="6">
         <v>3367</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="9">
@@ -4966,16 +4992,16 @@
         <v>39</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H54" s="6">
         <v>3</v>
       </c>
       <c r="I54" s="33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -4993,13 +5019,13 @@
         <v>42</v>
       </c>
       <c r="F55" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G55" s="28" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5014,21 +5040,21 @@
         <v>73</v>
       </c>
       <c r="F56" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G56" s="28" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H56" s="37">
         <v>1426</v>
       </c>
       <c r="I56" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="9">
@@ -5038,16 +5064,16 @@
         <v>39</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G57" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H57" s="6">
         <v>68</v>
       </c>
       <c r="I57" s="33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5062,7 +5088,7 @@
         <v>33</v>
       </c>
       <c r="F58" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I58" s="32" t="s">
         <v>4</v>
@@ -5080,7 +5106,7 @@
         <v>33</v>
       </c>
       <c r="F59" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H59" s="37">
         <v>2055</v>
@@ -5091,28 +5117,28 @@
     </row>
     <row r="60" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C60" s="8">
         <v>1983</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F60" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H60" s="6">
         <v>10</v>
       </c>
       <c r="I60" s="29" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5127,7 +5153,7 @@
         <v>33</v>
       </c>
       <c r="F61" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I61" s="32" t="s">
         <v>6</v>
@@ -5135,23 +5161,23 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="7">
         <v>2004</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F62" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H62" s="6">
         <v>16</v>
       </c>
       <c r="I62" s="33" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5166,10 +5192,10 @@
         <v>73</v>
       </c>
       <c r="F63" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G63" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I63" s="32" t="s">
         <v>72</v>
@@ -5187,7 +5213,7 @@
         <v>45</v>
       </c>
       <c r="F64" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G64" s="27" t="s">
         <v>46</v>
@@ -5196,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -5309,23 +5335,23 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5365,101 +5391,101 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
         <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
         <v>104</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
         <v>107</v>
-      </c>
-      <c r="B10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>109</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5516,43 +5542,43 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>